<commit_message>
Coreccion de ortrografia viaticos estimacion esfuerzo
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/1. Plantillas estimacion/Viaticos_q_Estimación_Esfuerzo.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/1. Plantillas estimacion/Viaticos_q_Estimación_Esfuerzo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="-105" windowWidth="8490" windowHeight="7425" tabRatio="711" activeTab="3"/>
+    <workbookView xWindow="6810" yWindow="-105" windowWidth="8490" windowHeight="7425" tabRatio="711" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="36" r:id="rId1"/>
@@ -115,7 +115,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Este es el factor historico que nos permite conocer aproximadamente cuanto tiempo en promedio toma desarrollar cada caso de uso en otros proyectos similares.
+Este es el factor histórico que nos permite conocer aproximadamente cuanto tiempo en promedio toma desarrollar cada caso de uso en otros proyectos similares.
 </t>
         </r>
       </text>
@@ -300,13 +300,7 @@
     <t>Dificultad del lenguaje de programación</t>
   </si>
   <si>
-    <t>Reuso</t>
-  </si>
-  <si>
     <t>Peso Ajustado</t>
-  </si>
-  <si>
-    <t>Categoria</t>
   </si>
   <si>
     <t>Total UCP:</t>
@@ -548,9 +542,6 @@
   </si>
   <si>
     <t>El factor de productividad es aquel que nos permite saber cuantas horas toma realizar un punto de caso de uso. Este factor debe ser tomado de datos históricos de proyectos similares.</t>
-  </si>
-  <si>
-    <t>La duración estimada en semanas nos sirve para calcular la cantidad de actividades de algunos workflows (flijos de trabajo) que son fijos y que dichas actividades son periódicas. Este valor será modificado conforme se tengan registros históricos de productividad por flujos de trabajo.</t>
   </si>
   <si>
     <r>
@@ -695,9 +686,6 @@
     <t>Implementación y validación</t>
   </si>
   <si>
-    <t>Costo de Analisis y Diseño</t>
-  </si>
-  <si>
     <t>Existen 8 factores ambientales estándar para estimar el impacto en la productividad de diversas cuestiones ambientales que tienen en una aplicación</t>
   </si>
   <si>
@@ -713,36 +701,18 @@
     <t>Administrador de la configuración</t>
   </si>
   <si>
-    <t>Verifcar casos de uso</t>
-  </si>
-  <si>
-    <t>Identificar riesgos ambientes y tecnicos que afectaran al proyecto</t>
-  </si>
-  <si>
     <t>Aprobar propuesta comercial</t>
   </si>
   <si>
-    <t>Ejectuar el proceso de riesgos</t>
-  </si>
-  <si>
-    <t>Estableer adaptaciones del proyecto</t>
-  </si>
-  <si>
     <t>Definir el plan de pruebas</t>
   </si>
   <si>
     <t>Definir la arquitectura del proyecto</t>
   </si>
   <si>
-    <t>Ejecutar el proceso toma de decisiónes</t>
-  </si>
-  <si>
     <t>Analizar y diseñar la arquitectura</t>
   </si>
   <si>
-    <t>Realizar la verificacipón de analisis y diseño</t>
-  </si>
-  <si>
     <t>Realizar validación del producto</t>
   </si>
   <si>
@@ -758,18 +728,6 @@
     <t>Manejo de usuarios</t>
   </si>
   <si>
-    <t>Administracion de proyectos y areas de proyectos</t>
-  </si>
-  <si>
-    <t>Administracion viaticos por proyecto</t>
-  </si>
-  <si>
-    <t>Administracion de gastos</t>
-  </si>
-  <si>
-    <t>Generacion de reportes</t>
-  </si>
-  <si>
     <t>Intermedio</t>
   </si>
   <si>
@@ -783,6 +741,48 @@
   </si>
   <si>
     <t xml:space="preserve">Verificación </t>
+  </si>
+  <si>
+    <t>Costo de Análisis y Diseño</t>
+  </si>
+  <si>
+    <t>Ejecutar el proceso toma de decisiones</t>
+  </si>
+  <si>
+    <t>Realizar la verificación de análisis y diseño</t>
+  </si>
+  <si>
+    <t>Verificar casos de uso</t>
+  </si>
+  <si>
+    <t>Identificar riesgos ambientes y técnicos que afectaran al proyecto</t>
+  </si>
+  <si>
+    <t>Ejecutar el proceso de riesgos</t>
+  </si>
+  <si>
+    <t>Establecer adaptaciones del proyecto</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Reusó</t>
+  </si>
+  <si>
+    <t>Administración de proyectos y áreas de proyectos</t>
+  </si>
+  <si>
+    <t>Administración viáticos por proyecto</t>
+  </si>
+  <si>
+    <t>Administración de gastos</t>
+  </si>
+  <si>
+    <t>Generación de reportes</t>
+  </si>
+  <si>
+    <t>La duración estimada en semanas nos sirve para calcular la cantidad de actividades de algunos workflows (flujos de trabajo) que son fijos y que dichas actividades son periódicas. Este valor será modificado conforme se tengan registros históricos de productividad por flujos de trabajo.</t>
   </si>
 </sst>
 </file>
@@ -2097,65 +2097,65 @@
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3099,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IV43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,11 +3114,11 @@
     <row r="2" spans="1:7" s="194" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="193"/>
       <c r="B2" s="214" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="214"/>
       <c r="D2" s="215" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E2" s="215"/>
       <c r="F2" s="215"/>
@@ -3127,7 +3127,7 @@
     <row r="4" spans="1:7" s="192" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="191"/>
       <c r="B4" s="195" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="191"/>
       <c r="D4" s="191"/>
@@ -3136,12 +3136,12 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>4</v>
@@ -3152,20 +3152,20 @@
         <v>9</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>10</v>
@@ -3174,7 +3174,7 @@
     <row r="12" spans="1:7" s="192" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="191"/>
       <c r="B12" s="195" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" s="191"/>
       <c r="D12" s="191"/>
@@ -3183,17 +3183,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>4</v>
@@ -3274,7 +3274,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:256" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>34</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D28" s="6"/>
     </row>
@@ -3316,7 +3316,7 @@
     <row r="31" spans="1:256" s="192" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A31" s="191"/>
       <c r="B31" s="195" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="191"/>
       <c r="D31" s="191"/>
@@ -3326,7 +3326,7 @@
     <row r="32" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3586,7 +3586,7 @@
     <row r="33" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -3845,7 +3845,7 @@
     </row>
     <row r="35" spans="1:256" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>4</v>
@@ -3880,7 +3880,7 @@
         <v>43</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:256" x14ac:dyDescent="0.25">
@@ -3936,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3955,44 +3955,44 @@
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="216" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="216"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="216"/>
+      <c r="B3" s="234" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="234"/>
+      <c r="F3" s="234"/>
+      <c r="G3" s="234"/>
+      <c r="H3" s="234"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="217" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="217"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="217"/>
-      <c r="G4" s="217"/>
-      <c r="H4" s="217"/>
+      <c r="B4" s="235" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="235"/>
+      <c r="F4" s="235"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="235"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="94"/>
     </row>
     <row r="8" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="220" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="221"/>
-      <c r="D8" s="221"/>
-      <c r="E8" s="221"/>
-      <c r="F8" s="221"/>
-      <c r="G8" s="221"/>
-      <c r="H8" s="222"/>
+      <c r="B8" s="229" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
+      <c r="G8" s="230"/>
+      <c r="H8" s="231"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="173"/>
@@ -4010,13 +4010,13 @@
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="176" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="177" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="178" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10" s="178" t="s">
         <v>3</v>
@@ -4024,10 +4024,10 @@
       <c r="F10" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="223" t="s">
+      <c r="G10" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="224"/>
+      <c r="H10" s="233"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -4046,8 +4046,8 @@
         <f t="shared" ref="F11:F23" si="0">E11*D11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="225"/>
-      <c r="H11" s="226"/>
+      <c r="G11" s="227"/>
+      <c r="H11" s="228"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4195,7 +4195,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D19" s="186">
         <v>1</v>
@@ -4255,7 +4255,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" s="186">
         <v>1</v>
@@ -4295,7 +4295,7 @@
       <c r="C24" s="180"/>
       <c r="D24" s="180"/>
       <c r="E24" s="180" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" s="181">
         <f>SUM(F11:F23)</f>
@@ -4305,15 +4305,15 @@
       <c r="H24" s="182"/>
     </row>
     <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="220" t="s">
+      <c r="B27" s="229" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="221"/>
-      <c r="D27" s="221"/>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221"/>
-      <c r="G27" s="221"/>
-      <c r="H27" s="222"/>
+      <c r="C27" s="230"/>
+      <c r="D27" s="230"/>
+      <c r="E27" s="230"/>
+      <c r="F27" s="230"/>
+      <c r="G27" s="230"/>
+      <c r="H27" s="231"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="174"/>
@@ -4331,13 +4331,13 @@
     </row>
     <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="176" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" s="177" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="178" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" s="178" t="s">
         <v>3</v>
@@ -4345,10 +4345,10 @@
       <c r="F29" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="223" t="s">
+      <c r="G29" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="224"/>
+      <c r="H29" s="233"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
@@ -4367,8 +4367,8 @@
         <f t="shared" ref="F30:F37" si="1">E30*D30</f>
         <v>4.5</v>
       </c>
-      <c r="G30" s="225"/>
-      <c r="H30" s="226"/>
+      <c r="G30" s="227"/>
+      <c r="H30" s="228"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
@@ -4415,7 +4415,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D33" s="184">
         <v>0.5</v>
@@ -4515,7 +4515,7 @@
       <c r="C38" s="188"/>
       <c r="D38" s="180"/>
       <c r="E38" s="188" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F38" s="181">
         <f>SUM(F30:F37)</f>
@@ -4525,44 +4525,56 @@
       <c r="H38" s="182"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="229" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="230"/>
-      <c r="F40" s="233" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" s="234"/>
-      <c r="H40" s="234"/>
+      <c r="B40" s="220" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="221"/>
+      <c r="F40" s="224" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="225"/>
+      <c r="H40" s="225"/>
     </row>
     <row r="41" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="231" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" s="232"/>
-      <c r="F41" s="231" t="s">
-        <v>136</v>
-      </c>
-      <c r="G41" s="235"/>
-      <c r="H41" s="235"/>
+      <c r="B41" s="222" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="223"/>
+      <c r="F41" s="222" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="226"/>
+      <c r="H41" s="226"/>
     </row>
     <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="190" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C42" s="213">
         <v>15</v>
       </c>
       <c r="F42" s="189" t="s">
-        <v>67</v>
-      </c>
-      <c r="G42" s="227">
+        <v>65</v>
+      </c>
+      <c r="G42" s="216">
         <v>0</v>
       </c>
-      <c r="H42" s="228"/>
+      <c r="H42" s="217"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B40:C40"/>
@@ -4579,18 +4591,6 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G29:H29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -4609,7 +4609,7 @@
   <dimension ref="B2:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4642,7 +4642,7 @@
       <c r="D3" s="170"/>
       <c r="E3" s="170"/>
       <c r="F3" s="170" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" s="171">
         <f>SUM(G5:G29)*'Factor de complejidad Téc y Amb'!H9*'Factor de complejidad Téc y Amb'!H28</f>
@@ -4657,16 +4657,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="168" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="E4" s="168" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="F4" s="168" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="168" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -4674,13 +4674,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F5" s="50">
         <f>IF(D5="Simple",5,IF(D5="Promedio",10,IF(D5="Complejo",15,0)))</f>
@@ -4696,13 +4696,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F6" s="50">
         <f t="shared" ref="F6:F29" si="1">IF(D6="Simple",5,IF(D6="Promedio",10,IF(D6="Complejo",15,0)))</f>
@@ -4718,13 +4718,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F7" s="50">
         <f t="shared" si="1"/>
@@ -4740,13 +4740,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F8" s="50">
         <f>IF(D8="Simple",5,IF(D8="Intermedio",10,IF(D8="Complejo",15,0)))</f>
@@ -4762,13 +4762,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F9" s="50">
         <f t="shared" ref="F9:F16" si="2">IF(D9="Simple",5,IF(D9="Intermedio",10,IF(D9="Complejo",15,0)))</f>
@@ -4784,7 +4784,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
@@ -4802,7 +4802,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
@@ -4820,7 +4820,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
@@ -4838,7 +4838,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
@@ -4856,7 +4856,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
@@ -4874,7 +4874,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
@@ -4892,7 +4892,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
@@ -4910,7 +4910,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
@@ -4928,7 +4928,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="130" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
@@ -4946,7 +4946,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="130" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
@@ -4964,7 +4964,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="130" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="20"/>
@@ -4982,7 +4982,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="20"/>
@@ -5000,7 +5000,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="20"/>
@@ -5018,7 +5018,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="20"/>
@@ -5036,7 +5036,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="20"/>
@@ -5054,7 +5054,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="20"/>
@@ -5170,8 +5170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5210,14 +5210,14 @@
     <row r="2" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23"/>
       <c r="C2" s="104" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D2" s="110">
         <f>'Estimación de Tamaño UCP'!G3</f>
         <v>26.891999999999996</v>
       </c>
       <c r="E2" s="105" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
@@ -5234,13 +5234,13 @@
     <row r="3" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="23"/>
       <c r="C3" s="106" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="103" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="107" t="s">
         <v>149</v>
-      </c>
-      <c r="D3" s="103" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" s="107" t="s">
-        <v>152</v>
       </c>
       <c r="F3" s="23">
         <f>'Factor de complejidad Téc y Amb'!C42</f>
@@ -5260,14 +5260,14 @@
     <row r="4" spans="2:16" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="23"/>
       <c r="C4" s="108" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D4" s="111">
         <f>D3*D2</f>
         <v>403.37999999999994</v>
       </c>
       <c r="E4" s="109" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -5300,7 +5300,7 @@
     </row>
     <row r="6" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="241" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="242"/>
       <c r="D6" s="242"/>
@@ -5332,31 +5332,31 @@
         <v>0</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="53" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H8" s="53" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="88" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J8" s="89" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K8" s="116" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -5378,7 +5378,7 @@
       <c r="G9" s="150"/>
       <c r="H9" s="157"/>
       <c r="I9" s="237" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J9" s="238"/>
       <c r="K9" s="203">
@@ -5389,7 +5389,7 @@
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="55"/>
       <c r="C10" s="196" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="77"/>
@@ -5404,7 +5404,7 @@
         <v>0.2413793103448276</v>
       </c>
       <c r="I10" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J10" s="91">
         <f>IF(I10="Líder de proyecto",[5]Recursos!E$5,(IF(I10="Analista",[5]Recursos!E$6,(IF(I10="Diseñador",[5]Recursos!#REF!,(IF(I10="Tester",[5]Recursos!E$7,(IF(I10="Desarrollador",[5]Recursos!E$8,(IF(I10="Arquitecto",[5]Recursos!E$12,(IF(I10="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5418,7 +5418,7 @@
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="55"/>
       <c r="C11" s="196" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="77"/>
@@ -5433,7 +5433,7 @@
         <v>0.10344827586206896</v>
       </c>
       <c r="I11" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J11" s="91">
         <f>IF(I11="Líder de proyecto",[5]Recursos!E$5,(IF(I11="Analista",[5]Recursos!E$6,(IF(I11="Diseñador",[5]Recursos!#REF!,(IF(I11="Tester",[5]Recursos!E$7,(IF(I11="Desarrollador",[5]Recursos!E$8,(IF(I11="Arquitecto",[5]Recursos!E$12,(IF(I11="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5447,7 +5447,7 @@
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="55"/>
       <c r="C12" s="196" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="77"/>
@@ -5462,7 +5462,7 @@
         <v>6.8965517241379309E-2</v>
       </c>
       <c r="I12" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J12" s="91">
         <f>IF(I12="Líder de proyecto",[5]Recursos!E$5,(IF(I12="Analista",[5]Recursos!E$6,(IF(I12="Diseñador",[5]Recursos!#REF!,(IF(I12="Tester",[5]Recursos!E$7,(IF(I12="Desarrollador",[5]Recursos!E$8,(IF(I12="Arquitecto",[5]Recursos!E$12,(IF(I12="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5476,7 +5476,7 @@
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="55"/>
       <c r="C13" s="196" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" s="55"/>
       <c r="E13" s="77"/>
@@ -5491,7 +5491,7 @@
         <v>0.41379310344827586</v>
       </c>
       <c r="I13" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J13" s="91">
         <f>IF(I13="Líder de proyecto",[5]Recursos!E$5,(IF(I13="Analista",[5]Recursos!E$6,(IF(I13="Diseñador",[5]Recursos!#REF!,(IF(I13="Tester",[5]Recursos!E$7,(IF(I13="Desarrollador",[5]Recursos!E$8,(IF(I13="Arquitecto",[5]Recursos!E$12,(IF(I13="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5505,7 +5505,7 @@
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="55"/>
       <c r="C14" s="196" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="77"/>
@@ -5520,7 +5520,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
       <c r="I14" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J14" s="91">
         <f>IF(I14="Líder de proyecto",[5]Recursos!E$5,(IF(I14="Analista",[5]Recursos!E$6,(IF(I14="Diseñador",[5]Recursos!#REF!,(IF(I14="Tester",[5]Recursos!E$7,(IF(I14="Desarrollador",[5]Recursos!E$8,(IF(I14="Arquitecto",[5]Recursos!E$12,(IF(I14="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5534,7 +5534,7 @@
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="55"/>
       <c r="C15" s="196" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="55"/>
       <c r="E15" s="197"/>
@@ -5549,7 +5549,7 @@
         <v>0.13793103448275862</v>
       </c>
       <c r="I15" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J15" s="91">
         <f>IF(I15="Líder de proyecto",[5]Recursos!E$5,(IF(I15="Analista",[5]Recursos!E$6,(IF(I15="Diseñador",[5]Recursos!#REF!,(IF(I15="Tester",[5]Recursos!E$7,(IF(I15="Desarrollador",[5]Recursos!E$8,(IF(I15="Arquitecto",[5]Recursos!E$12,(IF(I15="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5565,7 +5565,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="146" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="147"/>
       <c r="E16" s="152">
@@ -5579,10 +5579,10 @@
       <c r="G16" s="150"/>
       <c r="H16" s="157"/>
       <c r="I16" s="244" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J16" s="245" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K16" s="203">
         <f>SUM(K17+K25)</f>
@@ -5592,7 +5592,7 @@
     <row r="17" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="55"/>
       <c r="C17" s="66" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D17" s="79"/>
       <c r="E17" s="77"/>
@@ -5603,10 +5603,10 @@
       <c r="G17" s="80"/>
       <c r="H17" s="81"/>
       <c r="I17" s="246" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J17" s="247" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K17" s="204">
         <f>SUM(K18:K24)</f>
@@ -5616,7 +5616,7 @@
     <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="55"/>
       <c r="C18" s="196" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D18" s="55"/>
       <c r="E18" s="77"/>
@@ -5631,7 +5631,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
       <c r="I18" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J18" s="91">
         <f>IF(I18="Líder de proyecto",[5]Recursos!E$5,(IF(I18="Analista",[5]Recursos!E$6,(IF(I18="Diseñador",[5]Recursos!#REF!,(IF(I18="Tester",[5]Recursos!E$7,(IF(I18="Desarrollador",[5]Recursos!E$8,(IF(I18="Arquitecto",[5]Recursos!E$12,(IF(I18="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5645,7 +5645,7 @@
     <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="55"/>
       <c r="C19" s="196" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D19" s="55"/>
       <c r="E19" s="77"/>
@@ -5660,7 +5660,7 @@
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="I19" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J19" s="91">
         <f>IF(I19="Líder de proyecto",[5]Recursos!E$5,(IF(I19="Analista",[5]Recursos!E$6,(IF(I19="Diseñador",[5]Recursos!#REF!,(IF(I19="Tester",[5]Recursos!E$7,(IF(I19="Desarrollador",[5]Recursos!E$8,(IF(I19="Arquitecto",[5]Recursos!E$12,(IF(I19="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5674,7 +5674,7 @@
     <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="55"/>
       <c r="C20" s="196" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="55"/>
       <c r="E20" s="77"/>
@@ -5689,7 +5689,7 @@
         <v>0.13043478260869565</v>
       </c>
       <c r="I20" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J20" s="91">
         <f>IF(I20="Líder de proyecto",[5]Recursos!E$5,(IF(I20="Analista",[5]Recursos!E$6,(IF(I20="Diseñador",[5]Recursos!#REF!,(IF(I20="Tester",[5]Recursos!E$7,(IF(I20="Desarrollador",[5]Recursos!E$8,(IF(I20="Arquitecto",[5]Recursos!E$12,(IF(I20="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5703,7 +5703,7 @@
     <row r="21" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="55"/>
       <c r="C21" s="196" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="77"/>
@@ -5718,7 +5718,7 @@
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="I21" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J21" s="91">
         <f>IF(I21="Líder de proyecto",[5]Recursos!E$5,(IF(I21="Analista",[5]Recursos!E$6,(IF(I21="Diseñador",[5]Recursos!#REF!,(IF(I21="Tester",[5]Recursos!E$7,(IF(I21="Desarrollador",[5]Recursos!E$8,(IF(I21="Arquitecto",[5]Recursos!E$12,(IF(I21="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5733,7 +5733,7 @@
     <row r="22" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="55"/>
       <c r="C22" s="196" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D22" s="55"/>
       <c r="E22" s="77"/>
@@ -5748,7 +5748,7 @@
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="I22" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J22" s="91">
         <f>IF(I22="Líder de proyecto",[5]Recursos!E$5,(IF(I22="Analista",[5]Recursos!E$6,(IF(I22="Diseñador",[5]Recursos!#REF!,(IF(I22="Tester",[5]Recursos!E$7,(IF(I22="Desarrollador",[5]Recursos!E$8,(IF(I22="Arquitecto",[5]Recursos!E$12,(IF(I22="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5763,7 +5763,7 @@
     <row r="23" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="55"/>
       <c r="C23" s="196" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="D23" s="55"/>
       <c r="E23" s="77"/>
@@ -5778,7 +5778,7 @@
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="I23" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J23" s="91">
         <f>IF(I23="Líder de proyecto",[5]Recursos!E$5,(IF(I23="Analista",[5]Recursos!E$6,(IF(I23="Diseñador",[5]Recursos!#REF!,(IF(I23="Tester",[5]Recursos!E$7,(IF(I23="Desarrollador",[5]Recursos!E$8,(IF(I23="Arquitecto",[5]Recursos!E$12,(IF(I23="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5792,7 +5792,7 @@
     <row r="24" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="55"/>
       <c r="C24" s="198" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="D24" s="55"/>
       <c r="E24" s="77"/>
@@ -5807,7 +5807,7 @@
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="I24" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J24" s="91">
         <f>IF(I24="Líder de proyecto",[5]Recursos!E$5,(IF(I24="Analista",[5]Recursos!E$6,(IF(I24="Diseñador",[5]Recursos!#REF!,(IF(I24="Tester",[5]Recursos!E$7,(IF(I24="Desarrollador",[5]Recursos!E$8,(IF(I24="Arquitecto",[5]Recursos!E$12,(IF(I24="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5821,7 +5821,7 @@
     <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="55"/>
       <c r="C25" s="66" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D25" s="79"/>
       <c r="E25" s="77"/>
@@ -5832,10 +5832,10 @@
       <c r="G25" s="80"/>
       <c r="H25" s="81"/>
       <c r="I25" s="246" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J25" s="247" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K25" s="204">
         <f>SUM(K26:K29)</f>
@@ -5845,7 +5845,7 @@
     <row r="26" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="199"/>
       <c r="C26" s="196" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E26" s="77"/>
       <c r="F26" s="59">
@@ -5859,7 +5859,7 @@
         <v>0.2391304347826087</v>
       </c>
       <c r="I26" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J26" s="91">
         <f>IF(I26="Líder de proyecto",[5]Recursos!E$5,(IF(I26="Analista",[5]Recursos!E$6,(IF(I26="Diseñador",[5]Recursos!#REF!,(IF(I26="Tester",[5]Recursos!E$7,(IF(I26="Desarrollador",[5]Recursos!E$8,(IF(I26="Arquitecto",[5]Recursos!E$12,(IF(I26="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5873,7 +5873,7 @@
     <row r="27" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="55"/>
       <c r="C27" s="196" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D27" s="55"/>
       <c r="E27" s="77"/>
@@ -5888,7 +5888,7 @@
         <v>0.28260869565217389</v>
       </c>
       <c r="I27" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J27" s="91">
         <f>IF(I27="Líder de proyecto",[5]Recursos!E$5,(IF(I27="Analista",[5]Recursos!E$6,(IF(I27="Diseñador",[5]Recursos!#REF!,(IF(I27="Tester",[5]Recursos!E$7,(IF(I27="Desarrollador",[5]Recursos!E$8,(IF(I27="Arquitecto",[5]Recursos!E$12,(IF(I27="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5902,7 +5902,7 @@
     <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="55"/>
       <c r="C28" s="196" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="D28" s="55"/>
       <c r="E28" s="77"/>
@@ -5917,7 +5917,7 @@
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="I28" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J28" s="91">
         <f>IF(I28="Líder de proyecto",[5]Recursos!E$5,(IF(I28="Analista",[5]Recursos!E$6,(IF(I28="Diseñador",[5]Recursos!#REF!,(IF(I28="Tester",[5]Recursos!E$7,(IF(I28="Desarrollador",[5]Recursos!E$8,(IF(I28="Arquitecto",[5]Recursos!E$12,(IF(I28="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5931,7 +5931,7 @@
     <row r="29" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="55"/>
       <c r="C29" s="196" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D29" s="55"/>
       <c r="E29" s="197"/>
@@ -5946,7 +5946,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
       <c r="I29" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J29" s="91">
         <f>IF(I29="Líder de proyecto",[5]Recursos!E$5,(IF(I29="Analista",[5]Recursos!E$6,(IF(I29="Diseñador",[5]Recursos!#REF!,(IF(I29="Tester",[5]Recursos!E$7,(IF(I29="Desarrollador",[5]Recursos!E$8,(IF(I29="Arquitecto",[5]Recursos!E$12,(IF(I29="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -5962,7 +5962,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="146" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D30" s="153"/>
       <c r="E30" s="154">
@@ -5976,10 +5976,10 @@
       <c r="G30" s="150"/>
       <c r="H30" s="156"/>
       <c r="I30" s="237" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J30" s="238" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K30" s="203">
         <f>SUM(K38+K36+K44+K31)</f>
@@ -5991,7 +5991,7 @@
         <v>3.1</v>
       </c>
       <c r="C31" s="67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D31" s="68"/>
       <c r="E31" s="114">
@@ -6005,10 +6005,10 @@
       <c r="G31" s="78"/>
       <c r="H31" s="92"/>
       <c r="I31" s="248" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="J31" s="249" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K31" s="205">
         <f>SUM(K32:K35)</f>
@@ -6018,7 +6018,7 @@
     <row r="32" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="63"/>
       <c r="C32" s="196" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D32" s="57"/>
       <c r="E32" s="77"/>
@@ -6033,7 +6033,7 @@
         <v>0.04</v>
       </c>
       <c r="I32" s="90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J32" s="91">
         <f>IF(I32="Líder de proyecto",[5]Recursos!E$5,(IF(I32="Analista",[5]Recursos!E$6,(IF(I32="Diseñador",[5]Recursos!#REF!,(IF(I32="Tester",[5]Recursos!E$7,(IF(I32="Desarrollador",[5]Recursos!E$8,(IF(I32="Arquitecto",[5]Recursos!E$12,(IF(I32="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6047,7 +6047,7 @@
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="63"/>
       <c r="C33" s="196" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D33" s="57"/>
       <c r="E33" s="77"/>
@@ -6062,7 +6062,7 @@
         <v>0.03</v>
       </c>
       <c r="I33" s="90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J33" s="91">
         <f>IF(I33="Líder de proyecto",[5]Recursos!E$5,(IF(I33="Analista",[5]Recursos!E$6,(IF(I33="Diseñador",[5]Recursos!#REF!,(IF(I33="Tester",[5]Recursos!E$7,(IF(I33="Desarrollador",[5]Recursos!E$8,(IF(I33="Arquitecto",[5]Recursos!E$12,(IF(I33="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6076,7 +6076,7 @@
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="63"/>
       <c r="C34" s="196" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D34" s="57"/>
       <c r="E34" s="77"/>
@@ -6091,7 +6091,7 @@
         <v>0.04</v>
       </c>
       <c r="I34" s="90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J34" s="91">
         <f>IF(I34="Líder de proyecto",[5]Recursos!E$5,(IF(I34="Analista",[5]Recursos!E$6,(IF(I34="Diseñador",[5]Recursos!#REF!,(IF(I34="Tester",[5]Recursos!E$7,(IF(I34="Desarrollador",[5]Recursos!E$8,(IF(I34="Arquitecto",[5]Recursos!E$12,(IF(I34="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6105,7 +6105,7 @@
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="63"/>
       <c r="C35" s="196" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D35" s="57"/>
       <c r="E35" s="77"/>
@@ -6120,7 +6120,7 @@
         <v>0.02</v>
       </c>
       <c r="I35" s="90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J35" s="91">
         <f>IF(I35="Líder de proyecto",[5]Recursos!E$5,(IF(I35="Analista",[5]Recursos!E$6,(IF(I35="Diseñador",[5]Recursos!#REF!,(IF(I35="Tester",[5]Recursos!E$7,(IF(I35="Desarrollador",[5]Recursos!E$8,(IF(I35="Arquitecto",[5]Recursos!E$12,(IF(I35="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6136,7 +6136,7 @@
         <v>3.2</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D36" s="68"/>
       <c r="E36" s="114">
@@ -6150,10 +6150,10 @@
       <c r="G36" s="78"/>
       <c r="H36" s="70"/>
       <c r="I36" s="248" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J36" s="249" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K36" s="205">
         <f>SUM(K37:K37)</f>
@@ -6163,7 +6163,7 @@
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="63"/>
       <c r="C37" s="56" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D37" s="57"/>
       <c r="E37" s="112"/>
@@ -6178,7 +6178,7 @@
         <v>0.65</v>
       </c>
       <c r="I37" s="90" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J37" s="91">
         <f>IF(I37="Líder de proyecto",[5]Recursos!E$5,(IF(I37="Analista",[5]Recursos!E$6,(IF(I37="Diseñador",[5]Recursos!#REF!,(IF(I37="Tester",[5]Recursos!E$7,(IF(I37="Desarrollador",[5]Recursos!E$8,(IF(I37="Arquitecto",[5]Recursos!E$12,(IF(I37="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6194,7 +6194,7 @@
         <v>3.3</v>
       </c>
       <c r="C38" s="67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D38" s="71"/>
       <c r="E38" s="114">
@@ -6208,10 +6208,10 @@
       <c r="G38" s="78"/>
       <c r="H38" s="70"/>
       <c r="I38" s="248" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J38" s="249" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K38" s="205">
         <f>SUM(K39:K43)</f>
@@ -6221,7 +6221,7 @@
     <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="63"/>
       <c r="C39" s="196" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D39" s="58"/>
       <c r="E39" s="77"/>
@@ -6236,7 +6236,7 @@
         <v>0.03</v>
       </c>
       <c r="I39" s="90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J39" s="91">
         <f>IF(I39="Líder de proyecto",[5]Recursos!E$5,(IF(I39="Analista",[5]Recursos!E$6,(IF(I39="Diseñador",[5]Recursos!#REF!,(IF(I39="Tester",[5]Recursos!E$7,(IF(I39="Desarrollador",[5]Recursos!E$8,(IF(I39="Arquitecto",[5]Recursos!E$12,(IF(I39="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6250,7 +6250,7 @@
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="63"/>
       <c r="C40" s="196" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D40" s="58"/>
       <c r="E40" s="77"/>
@@ -6265,7 +6265,7 @@
         <v>0.03</v>
       </c>
       <c r="I40" s="90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J40" s="91">
         <f>IF(I40="Líder de proyecto",[5]Recursos!E$5,(IF(I40="Analista",[5]Recursos!E$6,(IF(I40="Diseñador",[5]Recursos!#REF!,(IF(I40="Tester",[5]Recursos!E$7,(IF(I40="Desarrollador",[5]Recursos!E$8,(IF(I40="Arquitecto",[5]Recursos!E$12,(IF(I40="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6279,7 +6279,7 @@
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="63"/>
       <c r="C41" s="196" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D41" s="58"/>
       <c r="E41" s="77"/>
@@ -6294,7 +6294,7 @@
         <v>0.03</v>
       </c>
       <c r="I41" s="90" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J41" s="91">
         <f>IF(I41="Líder de proyecto",[5]Recursos!E$5,(IF(I41="Analista",[5]Recursos!E$6,(IF(I41="Diseñador",[5]Recursos!#REF!,(IF(I41="Tester",[5]Recursos!E$7,(IF(I41="Desarrollador",[5]Recursos!E$8,(IF(I41="Arquitecto",[5]Recursos!E$12,(IF(I41="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6308,7 +6308,7 @@
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="63"/>
       <c r="C42" s="196" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="D42" s="58"/>
       <c r="E42" s="77"/>
@@ -6323,7 +6323,7 @@
         <v>0.04</v>
       </c>
       <c r="I42" s="90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J42" s="91">
         <f>IF(I42="Líder de proyecto",[5]Recursos!E$5,(IF(I42="Analista",[5]Recursos!E$6,(IF(I42="Diseñador",[5]Recursos!#REF!,(IF(I42="Tester",[5]Recursos!E$7,(IF(I42="Desarrollador",[5]Recursos!E$8,(IF(I42="Arquitecto",[5]Recursos!E$12,(IF(I42="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6338,7 +6338,7 @@
       <c r="A43" s="206"/>
       <c r="B43" s="207"/>
       <c r="C43" s="196" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="D43" s="208"/>
       <c r="E43" s="77"/>
@@ -6353,7 +6353,7 @@
         <v>0.01</v>
       </c>
       <c r="I43" s="90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J43" s="91">
         <f>IF(I43="Líder de proyecto",[5]Recursos!E$5,(IF(I43="Analista",[5]Recursos!E$6,(IF(I43="Diseñador",[5]Recursos!#REF!,(IF(I43="Tester",[5]Recursos!E$7,(IF(I43="Desarrollador",[5]Recursos!E$8,(IF(I43="Arquitecto",[5]Recursos!E$12,(IF(I43="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6369,7 +6369,7 @@
         <v>3.4</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D44" s="69"/>
       <c r="E44" s="211">
@@ -6383,10 +6383,10 @@
       <c r="G44" s="78"/>
       <c r="H44" s="100"/>
       <c r="I44" s="248" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J44" s="249" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K44" s="205">
         <f>SUM(K45:K46)</f>
@@ -6396,7 +6396,7 @@
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="63"/>
       <c r="C45" s="56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D45" s="55"/>
       <c r="E45" s="77"/>
@@ -6410,7 +6410,7 @@
         <v>0.5</v>
       </c>
       <c r="I45" s="90" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J45" s="91">
         <f>IF(I45="Líder de proyecto",[5]Recursos!E$5,(IF(I45="Analista",[5]Recursos!E$6,(IF(I45="Diseñador",[5]Recursos!#REF!,(IF(I45="Tester",[5]Recursos!E$7,(IF(I45="Desarrollador",[5]Recursos!E$8,(IF(I45="Arquitecto",[5]Recursos!E$12,(IF(I45="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6424,7 +6424,7 @@
     <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="63"/>
       <c r="C46" s="56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D46" s="55"/>
       <c r="E46" s="77"/>
@@ -6438,7 +6438,7 @@
         <v>0.5</v>
       </c>
       <c r="I46" s="90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J46" s="91">
         <f>IF(I46="Líder de proyecto",[5]Recursos!E$5,(IF(I46="Analista",[5]Recursos!E$6,(IF(I46="Diseñador",[5]Recursos!#REF!,(IF(I46="Tester",[5]Recursos!E$7,(IF(I46="Desarrollador",[5]Recursos!E$8,(IF(I46="Arquitecto",[5]Recursos!E$12,(IF(I46="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6454,7 +6454,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="146" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D47" s="147"/>
       <c r="E47" s="152">
@@ -6468,10 +6468,10 @@
       <c r="G47" s="150"/>
       <c r="H47" s="151"/>
       <c r="I47" s="237" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J47" s="238" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K47" s="203">
         <f>SUM(K48:K49)</f>
@@ -6480,10 +6480,10 @@
     </row>
     <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="55" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" s="196" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D48" s="55"/>
       <c r="E48" s="200"/>
@@ -6497,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J48" s="91">
         <f>IF(I48="Líder de proyecto",[5]Recursos!E$5,(IF(I48="Analista",[5]Recursos!E$6,(IF(I48="Diseñador",[5]Recursos!#REF!,(IF(I48="Tester",[5]Recursos!E$7,(IF(I48="Desarrollador",[5]Recursos!E$8,(IF(I48="Arquitecto",[5]Recursos!E$12,(IF(I48="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6511,7 +6511,7 @@
     <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="55"/>
       <c r="C49" s="196" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D49" s="55"/>
       <c r="E49" s="200"/>
@@ -6525,7 +6525,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J49" s="91">
         <f>IF(I49="Líder de proyecto",[5]Recursos!E$5,(IF(I49="Analista",[5]Recursos!E$6,(IF(I49="Diseñador",[5]Recursos!#REF!,(IF(I49="Tester",[5]Recursos!E$7,(IF(I49="Desarrollador",[5]Recursos!E$8,(IF(I49="Arquitecto",[5]Recursos!E$12,(IF(I49="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6541,7 +6541,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="146" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D50" s="147"/>
       <c r="E50" s="148">
@@ -6555,10 +6555,10 @@
       <c r="G50" s="150"/>
       <c r="H50" s="151"/>
       <c r="I50" s="237" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J50" s="238" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K50" s="203">
         <f>SUM(K51:K54)</f>
@@ -6568,7 +6568,7 @@
     <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="72"/>
       <c r="C51" s="123" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D51" s="124"/>
       <c r="E51" s="77"/>
@@ -6583,7 +6583,7 @@
         <v>0.30232558139534882</v>
       </c>
       <c r="I51" s="90" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J51" s="91">
         <f>IF(I51="Líder de proyecto",[5]Recursos!E$5,(IF(I51="Analista",[5]Recursos!E$6,(IF(I51="Administrador de la configuración",[5]Recursos!E$11,(IF(I51="Tester",[5]Recursos!E$7,(IF(I51="Desarrollador",[5]Recursos!E$8,(IF(I51="Arquitecto",[5]Recursos!E$12,(IF(I51="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6596,10 +6596,10 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C52" s="123" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D52" s="124"/>
       <c r="E52" s="77"/>
@@ -6614,7 +6614,7 @@
         <v>0.51162790697674421</v>
       </c>
       <c r="I52" s="90" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J52" s="91">
         <f>IF(I52="Líder de proyecto",[5]Recursos!E$5,(IF(I52="Analista",[5]Recursos!E$6,(IF(I52="Diseñador",[5]Recursos!#REF!,(IF(I52="Tester",[5]Recursos!E$7,(IF(I52="Desarrollador",[5]Recursos!E$8,(IF(I52="Arquitecto",[5]Recursos!E$12,(IF(I52="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6627,10 +6627,10 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C53" s="123" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D53" s="124"/>
       <c r="E53" s="77"/>
@@ -6645,7 +6645,7 @@
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="I53" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J53" s="91">
         <f>IF(I53="Líder de proyecto",[5]Recursos!E$5,(IF(I53="Analista",[5]Recursos!E$6,(IF(I53="Diseñador",[5]Recursos!#REF!,(IF(I53="Tester",[5]Recursos!E$7,(IF(I53="Desarrollador",[5]Recursos!E$8,(IF(I53="Arquitecto",[5]Recursos!E$12,(IF(I53="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6658,7 +6658,7 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="113" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="125" t="s">
         <v>8</v>
@@ -6676,7 +6676,7 @@
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="I54" s="90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J54" s="91">
         <f>IF(I54="Líder de proyecto",[5]Recursos!E$5,(IF(I54="Analista",[5]Recursos!E$6,(IF(I54="Diseñador",[5]Recursos!#REF!,(IF(I54="Tester",[5]Recursos!E$7,(IF(I54="Desarrollador",[5]Recursos!E$8,(IF(I54="Arquitecto",[5]Recursos!E$12,(IF(I54="Aseguramiento de la calidad",[5]Recursos!E$9,0)))))))))))))</f>
@@ -6694,7 +6694,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="138" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D55" s="139"/>
       <c r="E55" s="140"/>
@@ -6705,10 +6705,10 @@
         <v>1</v>
       </c>
       <c r="H55" s="143" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I55" s="237" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J55" s="238"/>
       <c r="K55" s="144">
@@ -6721,12 +6721,12 @@
       <c r="D56" s="6"/>
       <c r="E56" s="98"/>
       <c r="F56" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="239" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J56" s="239"/>
       <c r="K56" s="83">
@@ -6739,7 +6739,7 @@
       <c r="C57" s="64"/>
       <c r="D57" s="25"/>
       <c r="I57" s="161" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J57" s="162"/>
       <c r="K57" s="163">
@@ -6751,11 +6751,11 @@
       <c r="C58" s="64"/>
       <c r="D58" s="25"/>
       <c r="I58" s="158" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J58" s="159"/>
       <c r="K58" s="160" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -6798,10 +6798,10 @@
       <c r="C63" s="64"/>
       <c r="D63" s="25"/>
       <c r="I63" s="96" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J63" s="96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K63" s="97">
         <f>SUM(K56:K62)</f>
@@ -6812,10 +6812,10 @@
       <c r="C64" s="240"/>
       <c r="D64" s="240"/>
       <c r="I64" s="212" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K64" s="1">
         <v>1.1599999999999999</v>
@@ -6823,10 +6823,10 @@
     </row>
     <row r="65" spans="9:11" ht="21" x14ac:dyDescent="0.35">
       <c r="I65" s="96" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J65" s="96" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K65" s="93">
         <f>K63*K64</f>
@@ -6881,7 +6881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -6895,27 +6895,27 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="164" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="164" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="164" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="165" t="s">
         <v>91</v>
-      </c>
-      <c r="D4" s="164" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="165" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="121" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="84">
         <v>11788.65</v>
@@ -6931,7 +6931,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="121" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="84">
         <v>9785.6299999999992</v>
@@ -6947,7 +6947,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="121" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" s="84">
         <v>9785.6299999999992</v>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="134" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C8" s="84">
         <v>11788.65</v>
@@ -6979,7 +6979,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="134" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C9" s="84">
         <v>5009.28</v>
@@ -6995,7 +6995,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="121" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="84">
         <v>9176.4599999999991</v>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="134" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C11" s="84">
         <v>5009.28</v>
@@ -7027,7 +7027,7 @@
     </row>
     <row r="12" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="122" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C12" s="84">
         <v>11788.65</v>
@@ -7044,15 +7044,15 @@
     <row r="14" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="166" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="74" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" s="85">
         <v>2800</v>
@@ -7060,7 +7060,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C17" s="85">
         <v>1600</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" s="85">
         <v>1700</v>
@@ -7076,7 +7076,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="74" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C19" s="85">
         <v>12000</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="74" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="85">
         <v>1750</v>
@@ -7092,7 +7092,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="74" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21" s="85">
         <v>200</v>
@@ -7100,7 +7100,7 @@
     </row>
     <row r="22" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C22" s="85">
         <v>1800</v>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="23" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="76" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23" s="86">
         <f>SUM(C16:C22)</f>
@@ -7118,13 +7118,13 @@
     <row r="26" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="167" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" s="73">
         <v>8</v>
       </c>
       <c r="D27" s="167" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E27" s="87">
         <f>((C23/C27)/30/8)</f>
@@ -7137,34 +7137,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
-    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -7248,39 +7220,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
+    <Owner xmlns="035E5738-9077-49AA-867C-265905AEBD06">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7295,4 +7263,36 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>